<commit_message>
Documentation - new points
Added the Scenaries, test strategy, planification and updated the pictures of the Models and MCD
</commit_message>
<xml_diff>
--- a/Documentation/UseCases - Scénarios/Scénarios/ScénariosAdmin.xlsx
+++ b/Documentation/UseCases - Scénarios/Scénarios/ScénariosAdmin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel.PITTET\Documents\GitHub\Pre-TPI_2023\Documentation\UseCases - Scénarios\Scénarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864F9A4F-0C1F-4424-862D-61F26BA1526F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C46558-F06D-49D9-8A14-A74BB0F1B509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CC9808D-9F48-48C1-8654-DA68AC4A64CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3CC9808D-9F48-48C1-8654-DA68AC4A64CA}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD Intolerances" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
     <t>Action utilisateur</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Ajouter, modifier ou supprimer des allergies et intolérances</t>
   </si>
   <si>
-    <t>Clique sur le bouton &lt;admin&gt;</t>
-  </si>
-  <si>
     <t>Affiche la page de gestion administrateur</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Clique sur le bouton &lt;Modify&gt;</t>
   </si>
   <si>
-    <t>Modifie l'intolérance à la BDD</t>
-  </si>
-  <si>
     <t>Clique sur le bouton &lt;Delete&gt;</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Ajoute le plat à la BDD</t>
   </si>
   <si>
-    <t>Modifie le plat à la BDD</t>
-  </si>
-  <si>
     <t>Supprime le plat de la BDD</t>
   </si>
   <si>
@@ -116,10 +107,25 @@
     <t>Ajoute l'utilisateur à la BDD</t>
   </si>
   <si>
-    <t>Modifie l'utilisateur à la BDD</t>
-  </si>
-  <si>
     <t>Supprime l'utilisateur de la BDD</t>
+  </si>
+  <si>
+    <t>Oui --&gt;</t>
+  </si>
+  <si>
+    <t>Non --&gt;</t>
+  </si>
+  <si>
+    <t>Affiche un message d'erreur</t>
+  </si>
+  <si>
+    <t>Modifie le plat dans la BDD</t>
+  </si>
+  <si>
+    <t>Modifie l'intolérance dans la BDD</t>
+  </si>
+  <si>
+    <t>Modifie l'utilisateur dans la BDD</t>
   </si>
 </sst>
 </file>
@@ -651,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4912A2A7-110A-43DA-9D5A-628EDF5219BE}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,20 +686,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,78 +709,80 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -782,24 +790,40 @@
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -827,7 +851,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C19" sqref="A6:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +861,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -855,20 +879,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -878,78 +902,80 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -957,24 +983,40 @@
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1001,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C2BFF1-D369-412D-9557-51B2637A757B}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1054,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1030,20 +1072,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,78 +1095,80 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1132,24 +1176,40 @@
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>

</xml_diff>